<commit_message>
ref: backfilled rent_estimates, did more stuff
</commit_message>
<xml_diff>
--- a/Real Estate Investing.xlsx
+++ b/Real Estate Investing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armaangupta/Documents/Repositories/propdeals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160E997E-10D3-034C-84AB-B6D586F81D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABC6B7F-0ED8-5440-9B0C-BF44490E2279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="760" windowWidth="14980" windowHeight="18740" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2541,7 +2541,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2676,8 +2676,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="93" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3403,7 +3403,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4851,7 +4851,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5538,7 +5538,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6509,8 +6509,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7244,8 +7244,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="163" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7979,8 +7979,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="XEW10" zoomScale="125" workbookViewId="0">
-      <selection activeCell="XFD32" sqref="XFD32"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8714,8 +8714,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9449,8 +9449,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10196,8 +10196,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="AN25" sqref="AN25"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10931,8 +10931,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="137" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>